<commit_message>
ASKAPSDP-2884 updated SMS service and code generation to add int64 component ID to ICE results
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -14,6 +14,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -61,8 +62,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Collins, Daniel (IM&amp;T, Kensington WA):
-</t>
+          <t>Collins, Daniel (IM&amp;T, Kensington WA):</t>
         </r>
         <r>
           <rPr>
@@ -87,8 +87,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Collins, Daniel (IM&amp;T, Kensington WA):
-</t>
+          <t>Collins, Daniel (IM&amp;T, Kensington WA):</t>
         </r>
         <r>
           <rPr>
@@ -688,13 +687,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -717,6 +709,13 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -805,7 +804,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -818,47 +817,47 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -866,11 +865,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -882,7 +881,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,7 +889,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -898,15 +897,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -922,7 +921,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -934,7 +933,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -982,7 +981,7 @@
       <rgbColor rgb="FF9C6500"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1030,53 +1029,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1093320</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10017000" cy="9527040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1087,7 +1040,7 @@
   <dimension ref="1:37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12529,11 +12482,6 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F:K">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="false" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="F5:I37" type="whole">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
ASKAPSDP-2728 added new fields from the selavy component catalog. Updated tests, schema version, and slice files
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -5,18 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue description" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Comparison with Selavy" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Catalogue description'!$A$1:$L$37</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,7 +43,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t xml:space="preserve">Author:</t>
         </r>
         <r>
           <rPr>
@@ -47,7 +53,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Selects fields for inclusion in the data subset presented for LSM queries</t>
+          <t xml:space="preserve">Selects fields for inclusion in the data subset presented for LSM queries</t>
         </r>
       </text>
     </comment>
@@ -62,7 +68,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Collins, Daniel (IM&amp;T, Kensington WA):</t>
+          <t xml:space="preserve">Collins, Daniel (IM&amp;T, Kensington WA):</t>
         </r>
         <r>
           <rPr>
@@ -72,7 +78,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>If true, then an entry for this item is generated in the query criteria structure. This allows search criteria to be specified for the field when using the Ice API</t>
+          <t xml:space="preserve">If true, then an entry for this item is generated in the query criteria structure. This allows search criteria to be specified for the field when using the Ice API</t>
         </r>
       </text>
     </comment>
@@ -87,7 +93,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Collins, Daniel (IM&amp;T, Kensington WA):</t>
+          <t xml:space="preserve">Collins, Daniel (IM&amp;T, Kensington WA):</t>
         </r>
         <r>
           <rPr>
@@ -97,7 +103,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Indicates that negative values are invalid for the given field. This allows generation of a simpler search criteria API since negative values can be used to indicate an unused criteria. If this flag is true, then an additional boolean is generated.</t>
+          <t xml:space="preserve">Indicates that negative values are invalid for the given field. This allows generation of a simpler search criteria API since negative values can be used to indicate an unused criteria. If this flag is true, then an additional boolean is generated.</t>
         </r>
       </text>
     </comment>
@@ -106,553 +112,583 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="182">
-  <si>
-    <t>gsm.continuum_component 
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="192">
+  <si>
+    <t xml:space="preserve">gsm.continuum_component 
 10 November 2016</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ucd</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>datatype</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>include_in_gsm</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>nullable</t>
-  </si>
-  <si>
-    <t>lsm_view</t>
-  </si>
-  <si>
-    <t>generate_query_criteria</t>
-  </si>
-  <si>
-    <t>negative_is_invalid</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>observation_date</t>
-  </si>
-  <si>
-    <t>The observation date</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>Posix Date-time</t>
-  </si>
-  <si>
-    <t>For ASKAP sources, this is the date of the observation. For non-ASKAP sources, this field is NULL.</t>
-  </si>
-  <si>
-    <t>healpix_index</t>
-  </si>
-  <si>
-    <t>The HEALPix index of this component</t>
-  </si>
-  <si>
-    <t>BIGINT</t>
-  </si>
-  <si>
-    <t>sb_id</t>
-  </si>
-  <si>
-    <t>Scheduling Block identifier</t>
-  </si>
-  <si>
-    <t>component_id</t>
-  </si>
-  <si>
-    <t>meta.id;meta.main</t>
-  </si>
-  <si>
-    <t>Component identifier</t>
-  </si>
-  <si>
-    <t>VARCHAR</t>
-  </si>
-  <si>
-    <t>component_name</t>
-  </si>
-  <si>
-    <t>meta.id</t>
-  </si>
-  <si>
-    <t>Component name</t>
-  </si>
-  <si>
-    <t>Can be generated if required from ra_deg_cont and dec_deg_cont</t>
-  </si>
-  <si>
-    <t>ra_hms_cont</t>
-  </si>
-  <si>
-    <t>pos.eq.ra</t>
-  </si>
-  <si>
-    <t>J2000 right ascension (hh:mm:ss.sss)</t>
-  </si>
-  <si>
-    <t>h:m:s</t>
-  </si>
-  <si>
-    <t>dec_dms_cont</t>
-  </si>
-  <si>
-    <t>pos.eq.dec</t>
-  </si>
-  <si>
-    <t>J2000 declination (dd:mm:ss.ss)</t>
-  </si>
-  <si>
-    <t>deg:arcmin:arcsec</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
-    <t>pos.eq.ra;meta.main</t>
-  </si>
-  <si>
-    <t>J2000 right ascension</t>
-  </si>
-  <si>
-    <t>DOUBLE</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
-    <t>dec</t>
-  </si>
-  <si>
-    <t>pos.eq.dec;meta.main</t>
-  </si>
-  <si>
-    <t>J2000 declination</t>
-  </si>
-  <si>
-    <t>ra_err</t>
-  </si>
-  <si>
-    <t>stat.error;pos.eq.ra</t>
-  </si>
-  <si>
-    <t>Error in Right Ascension</t>
-  </si>
-  <si>
-    <t>REAL</t>
-  </si>
-  <si>
-    <t>arcsec</t>
-  </si>
-  <si>
-    <t>dec_err</t>
-  </si>
-  <si>
-    <t>stat.error;pos.eq.dec</t>
-  </si>
-  <si>
-    <t>Error in Declination</t>
-  </si>
-  <si>
-    <t>freq</t>
-  </si>
-  <si>
-    <t>em.freq</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>MHz</t>
-  </si>
-  <si>
-    <t>flux_peak</t>
-  </si>
-  <si>
-    <t>phot.flux.density;stat.max;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Peak flux density</t>
-  </si>
-  <si>
-    <t>mJy/beam</t>
-  </si>
-  <si>
-    <t>flux_peak_err</t>
-  </si>
-  <si>
-    <t>stat.error;phot.flux.density;stat.max;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Error in peak flux density</t>
-  </si>
-  <si>
-    <t>flux_int</t>
-  </si>
-  <si>
-    <t>phot.flux.density;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Integrated flux density</t>
-  </si>
-  <si>
-    <t>mJy</t>
-  </si>
-  <si>
-    <t>flux_int_err</t>
-  </si>
-  <si>
-    <t>stat.error;phot.flux.density;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Error in integrated flux density</t>
-  </si>
-  <si>
-    <t>maj_axis</t>
-  </si>
-  <si>
-    <t>phys.angSize.smajAxis;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>FWHM major axis before deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis</t>
-  </si>
-  <si>
-    <t>phys.angSize.sminAxis;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>FWHM minor axis before deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang</t>
-  </si>
-  <si>
-    <t>phys.angSize;pos.posAng;em.radio;stat.fit</t>
-  </si>
-  <si>
-    <t>Position angle before deconvolution</t>
-  </si>
-  <si>
-    <t>maj_axis_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize.smajAxis;em.radio</t>
-  </si>
-  <si>
-    <t>Error in major axis before deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize.sminAxis;em.radio</t>
-  </si>
-  <si>
-    <t>Error in minor axis before deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang_err</t>
-  </si>
-  <si>
-    <t>stat.error;phys.angSize;pos.posAng;em.radio</t>
-  </si>
-  <si>
-    <t>Error in position angle before deconvolution</t>
-  </si>
-  <si>
-    <t>maj_axis_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>FWHM major axis after deconvolution</t>
-  </si>
-  <si>
-    <t>min_axis_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>FWHM minor axis after deconvolution</t>
-  </si>
-  <si>
-    <t>pos_ang_deconv</t>
-  </si>
-  <si>
-    <t>phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
-  </si>
-  <si>
-    <t>Position angle after deconvolution</t>
-  </si>
-  <si>
-    <t>chi_squared_fit</t>
-  </si>
-  <si>
-    <t>stat.fit.chi2</t>
-  </si>
-  <si>
-    <t>Chi-squared value of Gaussian fit</t>
-  </si>
-  <si>
-    <t>rms_fit_Gauss</t>
-  </si>
-  <si>
-    <t>stat.stdev;stat.fit</t>
-  </si>
-  <si>
-    <t>RMS residual of Gaussian fit</t>
-  </si>
-  <si>
-    <t>spectral_index</t>
-  </si>
-  <si>
-    <t>spect.index;em.radio</t>
-  </si>
-  <si>
-    <t>Spectral index (First Taylor term)</t>
-  </si>
-  <si>
-    <t>spectral_curvature</t>
-  </si>
-  <si>
-    <t>askap:spect.curvature;em.radio</t>
-  </si>
-  <si>
-    <t>Spectral curvature (Second Taylor term)</t>
-  </si>
-  <si>
-    <t>rms_image</t>
-  </si>
-  <si>
-    <t>stat.stdev;phot.flux.density</t>
-  </si>
-  <si>
-    <t>rms noise level in image</t>
-  </si>
-  <si>
-    <t>has_siblings</t>
-  </si>
-  <si>
-    <t>meta.code</t>
-  </si>
-  <si>
-    <t>Source has siblings</t>
-  </si>
-  <si>
-    <t>BOOLEAN</t>
-  </si>
-  <si>
-    <t>fit_is_estimate</t>
-  </si>
-  <si>
-    <t>Component parameters are initial estimate, not from fit</t>
-  </si>
-  <si>
-    <t>flag_c3</t>
-  </si>
-  <si>
-    <t>Placeholder flag3</t>
-  </si>
-  <si>
-    <t>INTEGER</t>
-  </si>
-  <si>
-    <t>flag_c4</t>
-  </si>
-  <si>
-    <t>Placeholder flag4</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>meta.note</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
-    <t>Column order</t>
-  </si>
-  <si>
-    <t>CASDA Field Name</t>
-  </si>
-  <si>
-    <t>Associated Selavy Name</t>
-  </si>
-  <si>
-    <t>Selavy Unit</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>ii</t>
-  </si>
-  <si>
-    <t>catalogue_id</t>
-  </si>
-  <si>
-    <t>iii</t>
-  </si>
-  <si>
-    <t>iv</t>
-  </si>
-  <si>
-    <t>project_id</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>island_id</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Columns with a selavy name of none will be left empty. They will be provided in a future Selavy verison.</t>
-  </si>
-  <si>
-    <t>degdms_cont</t>
-  </si>
-  <si>
-    <t>ra_deg_cont</t>
-  </si>
-  <si>
-    <t>RA</t>
-  </si>
-  <si>
-    <t>dec_deg_cont</t>
-  </si>
-  <si>
-    <t>DEC</t>
-  </si>
-  <si>
-    <t>ra_deg_cont_err</t>
-  </si>
-  <si>
-    <t>dec_deg_cont_err</t>
-  </si>
-  <si>
-    <t>F_pk(fit)</t>
-  </si>
-  <si>
-    <t>Jy/beam</t>
-  </si>
-  <si>
-    <t>F_int(fit)</t>
-  </si>
-  <si>
-    <t>Jy</t>
-  </si>
-  <si>
-    <t>Maj(fit)</t>
-  </si>
-  <si>
-    <t>Min(fit)</t>
-  </si>
-  <si>
-    <t>P.A.(fit)</t>
-  </si>
-  <si>
-    <t>Maj(fit_deconv)</t>
-  </si>
-  <si>
-    <t>Min(fit_deconv)</t>
-  </si>
-  <si>
-    <t>P.A.(fit_deconv)</t>
-  </si>
-  <si>
-    <t>Chisq(fit)</t>
-  </si>
-  <si>
-    <t>RMS(fit)</t>
-  </si>
-  <si>
-    <t>RMS(image)</t>
-  </si>
-  <si>
-    <t>flag_c1</t>
-  </si>
-  <si>
-    <t>flag_c2</t>
-  </si>
-  <si>
-    <t>Other Selavy fields</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>F_peak</t>
-  </si>
-  <si>
-    <t>F_int</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Nfree(fit)</t>
-  </si>
-  <si>
-    <t>NDoF(fit)</t>
-  </si>
-  <si>
-    <t>Npix(fit)</t>
-  </si>
-  <si>
-    <t>Npix(obj)</t>
-  </si>
-  <si>
-    <t>Guess?</t>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ucd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datatype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include_in_gsm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nullable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lsm_view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generate_query_criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative_is_invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observation_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The observation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATETIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posix Date-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For ASKAP sources, this is the date of the observation. For non-ASKAP sources, this field is NULL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">healpix_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HEALPix index of this component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIGINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sb_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduling Block identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta.id;meta.main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be generated if required from ra_deg_cont and dec_deg_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra_hms_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos.eq.ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2000 right ascension (hh:mm:ss.sss)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h:m:s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dec_dms_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos.eq.dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2000 declination (dd:mm:ss.ss)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deg:arcmin:arcsec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos.eq.ra;meta.main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2000 right ascension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOUBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos.eq.dec;meta.main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2000 declination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;pos.eq.ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in Right Ascension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arcsec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dec_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;pos.eq.dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in Declination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">em.freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flux_peak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak flux density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mJy/beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flux_peak_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phot.flux.density;stat.max;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in peak flux density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flux_int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated flux density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mJy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flux_int_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phot.flux.density;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in integrated flux density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maj_axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize.smajAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWHM major axis before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize.sminAxis;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWHM minor axis before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_ang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize;pos.posAng;em.radio;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position angle before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maj_axis_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize.smajAxis;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in major axis before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_axis_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize.sminAxis;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in minor axis before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_ang_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize;pos.posAng;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in position angle before deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maj_axis_deconv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWHM major axis after deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_axis_deconv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWHM minor axis after deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_ang_deconv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position angle after deconvolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chi_squared_fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.fit.chi2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chi-squared value of Gaussian fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rms_fit_Gauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.stdev;stat.fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMS residual of Gaussian fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectral_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spect.index;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spectral index (First Taylor term)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectral_curvature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">askap:spect.curvature;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spectral curvature (Second Taylor term)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rms_image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.stdev;phot.flux.density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rms noise level in image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has_siblings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta.code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source has siblings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOLEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit_is_estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component parameters are initial estimate, not from fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag_c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder flag3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag_c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder flag4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta.note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">island_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meta.id.parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maj_axis_deconv_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize.smajAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_axis_deconv_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize.sminAxis;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_ang_deconv_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;phys.angSize;pos.posAng;em.radio;askap:meta.deconvolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectral_index_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stat.error;spect.index;em.radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectral_index_from_TT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASDA Field Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Associated Selavy Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selavy Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalogue_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns with a selavy name of none will be left empty. They will be provided in a future Selavy verison.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degdms_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra_deg_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dec_deg_cont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ra_deg_cont_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dec_deg_cont_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_pk(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jy/beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_int(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maj(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.A.(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maj(fit_deconv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min(fit_deconv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.A.(fit_deconv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chisq(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMS(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMS(image)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag_c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag_c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Selavy fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_peak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F_int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nfree(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NDoF(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Npix(fit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Npix(obj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guess?</t>
   </si>
 </sst>
 </file>
@@ -660,7 +696,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -933,34 +969,19 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
-        <sz val="11"/>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1037,26 +1058,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:37"/>
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="68.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.7142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="18"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="15"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="10"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="3" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="61.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="5" width="8.85714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="16.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="61.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="5" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3137,7 +3159,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
@@ -3173,7 +3195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
@@ -3205,7 +3227,7 @@
       </c>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="18" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
         <v>21</v>
       </c>
@@ -3238,7 +3260,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>23</v>
       </c>
@@ -4284,7 +4306,7 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
         <v>27</v>
       </c>
@@ -5332,7 +5354,7 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
@@ -6382,7 +6404,7 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
         <v>35</v>
       </c>
@@ -7432,7 +7454,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
         <v>39</v>
       </c>
@@ -8480,7 +8502,7 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
         <v>44</v>
       </c>
@@ -9528,7 +9550,7 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
         <v>47</v>
       </c>
@@ -10576,7 +10598,7 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
         <v>52</v>
       </c>
@@ -11624,7 +11646,7 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="18" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
         <v>55</v>
       </c>
@@ -11660,7 +11682,7 @@
       </c>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
         <v>59</v>
       </c>
@@ -11696,7 +11718,7 @@
       </c>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
         <v>63</v>
       </c>
@@ -11732,7 +11754,7 @@
       </c>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
@@ -11768,7 +11790,7 @@
       </c>
       <c r="L17" s="14"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
         <v>70</v>
       </c>
@@ -11804,7 +11826,7 @@
       </c>
       <c r="L18" s="14"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
         <v>73</v>
       </c>
@@ -11833,14 +11855,14 @@
         <v>1</v>
       </c>
       <c r="J19" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="22"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
         <v>76</v>
       </c>
@@ -11869,14 +11891,14 @@
         <v>1</v>
       </c>
       <c r="J20" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
         <v>79</v>
       </c>
@@ -11905,14 +11927,14 @@
         <v>1</v>
       </c>
       <c r="J21" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="15" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
         <v>82</v>
       </c>
@@ -11938,17 +11960,17 @@
         <v>0</v>
       </c>
       <c r="I22" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
         <v>85</v>
       </c>
@@ -11974,17 +11996,17 @@
         <v>0</v>
       </c>
       <c r="I23" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="22"/>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
         <v>88</v>
       </c>
@@ -12020,7 +12042,7 @@
       </c>
       <c r="L24" s="22"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
         <v>91</v>
       </c>
@@ -12056,7 +12078,7 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
         <v>94</v>
       </c>
@@ -12092,7 +12114,7 @@
       </c>
       <c r="L26" s="22"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
         <v>97</v>
       </c>
@@ -12128,7 +12150,7 @@
       </c>
       <c r="L27" s="22"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
         <v>100</v>
       </c>
@@ -12162,7 +12184,7 @@
       </c>
       <c r="L28" s="14"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
         <v>103</v>
       </c>
@@ -12198,7 +12220,7 @@
       </c>
       <c r="L29" s="14"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
         <v>106</v>
       </c>
@@ -12232,7 +12254,7 @@
       </c>
       <c r="L30" s="14"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
         <v>109</v>
       </c>
@@ -12266,7 +12288,7 @@
       </c>
       <c r="L31" s="14"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
         <v>112</v>
       </c>
@@ -12302,7 +12324,7 @@
       </c>
       <c r="L32" s="14"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
         <v>115</v>
       </c>
@@ -12336,7 +12358,7 @@
       </c>
       <c r="L33" s="14"/>
     </row>
-    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
         <v>119</v>
       </c>
@@ -12370,7 +12392,7 @@
       </c>
       <c r="L34" s="14"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
         <v>121</v>
       </c>
@@ -12404,7 +12426,7 @@
       </c>
       <c r="L35" s="14"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
         <v>124</v>
       </c>
@@ -12438,7 +12460,7 @@
       </c>
       <c r="L36" s="14"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
         <v>126</v>
       </c>
@@ -12472,13 +12494,246 @@
       </c>
       <c r="L37" s="14"/>
     </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L37"/>
+  <autoFilter ref="A1:L43"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:K499">
+  <conditionalFormatting sqref="F3:F499 G3:K38 G41:K499">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K39">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12490,7 +12745,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12507,18 +12762,18 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="1:1 C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="61.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.85714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="61.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12526,19 +12781,19 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12550,76 +12805,76 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E8" s="16"/>
     </row>
@@ -12638,10 +12893,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E10" s="16"/>
     </row>
@@ -12653,10 +12908,10 @@
         <v>27</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E11" s="16"/>
     </row>
@@ -12668,11 +12923,11 @@
         <v>31</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="16" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12680,10 +12935,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>137</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="16"/>
@@ -12693,10 +12948,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>43</v>
@@ -12708,10 +12963,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>43</v>
@@ -12723,10 +12978,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="16"/>
@@ -12736,10 +12991,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="16"/>
@@ -12752,10 +13007,10 @@
         <v>59</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E18" s="16"/>
     </row>
@@ -12767,7 +13022,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="16"/>
@@ -12780,10 +13035,10 @@
         <v>66</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -12795,7 +13050,7 @@
         <v>70</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="16"/>
@@ -12808,7 +13063,7 @@
         <v>73</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>51</v>
@@ -12823,7 +13078,7 @@
         <v>76</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>51</v>
@@ -12838,7 +13093,7 @@
         <v>79</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>43</v>
@@ -12853,7 +13108,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>51</v>
@@ -12868,7 +13123,7 @@
         <v>94</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>51</v>
@@ -12883,7 +13138,7 @@
         <v>97</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>43</v>
@@ -12898,10 +13153,10 @@
         <v>100</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E28" s="16"/>
     </row>
@@ -12913,7 +13168,7 @@
         <v>103</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>62</v>
@@ -12928,7 +13183,7 @@
         <v>106</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="16"/>
@@ -12941,7 +13196,7 @@
         <v>109</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="16"/>
@@ -12954,10 +13209,10 @@
         <v>112</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E32" s="16"/>
     </row>
@@ -12966,10 +13221,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="16"/>
@@ -12979,10 +13234,10 @@
         <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="16"/>
@@ -12995,7 +13250,7 @@
         <v>121</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="16"/>
@@ -13008,7 +13263,7 @@
         <v>124</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="16"/>
@@ -13021,7 +13276,7 @@
         <v>126</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="16"/>
@@ -13034,7 +13289,7 @@
         <v>82</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="16"/>
@@ -13047,7 +13302,7 @@
         <v>85</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="16"/>
@@ -13060,75 +13315,75 @@
         <v>88</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="16"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D41" s="28" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D43" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D45" s="0" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D46" s="0" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="0" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="0" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D49" s="0" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="0" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D52" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>